<commit_message>
them image vao cau hoi
</commit_message>
<xml_diff>
--- a/NhapCauHoi.xlsx
+++ b/NhapCauHoi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\Visual_Code\DoAnTotNghiep2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DoAn_2025\QuizzCenter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5BBBC4-9B8D-46FF-956E-5C01F24B010B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24EE4A2-1C41-4DBA-A073-80B6875D106C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2412" yWindow="1764" windowWidth="17280" windowHeight="9420" xr2:uid="{BE0AC574-4B40-4236-9B6A-98763779083F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BE0AC574-4B40-4236-9B6A-98763779083F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>Đáp án H</t>
   </si>
   <si>
-    <t>abc</t>
-  </si>
-  <si>
     <t>2+2</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>SFDS</t>
-  </si>
-  <si>
     <t>fdsaf</t>
   </si>
   <si>
@@ -112,6 +106,12 @@
   </si>
   <si>
     <t>Đáp án đúng</t>
+  </si>
+  <si>
+    <t>haha</t>
+  </si>
+  <si>
+    <t>hohoh</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -493,7 +493,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -522,19 +522,19 @@
     </row>
     <row r="2" spans="1:13" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
       </c>
       <c r="F2">
         <v>4</v>
@@ -551,34 +551,34 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
         <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Thêm câu hỏi vào đề bằng cách thủ công
</commit_message>
<xml_diff>
--- a/NhapCauHoi.xlsx
+++ b/NhapCauHoi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DoAn_2025\QuizzCenter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\Visual_Code\DoAnTotNghiep2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24EE4A2-1C41-4DBA-A073-80B6875D106C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85214E75-190F-4F94-A452-13A95E272571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BE0AC574-4B40-4236-9B6A-98763779083F}"/>
+    <workbookView xWindow="2412" yWindow="1764" windowWidth="17280" windowHeight="9420" xr2:uid="{BE0AC574-4B40-4236-9B6A-98763779083F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,10 +108,10 @@
     <t>Đáp án đúng</t>
   </si>
   <si>
-    <t>haha</t>
-  </si>
-  <si>
-    <t>hohoh</t>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test32</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -522,7 +522,7 @@
     </row>
     <row r="2" spans="1:13" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>16</v>

</xml_diff>